<commit_message>
Sprint Review Protocol 2 updated
</commit_message>
<xml_diff>
--- a/docs/reviews/Sprint_Review_Protocol_2.xlsx
+++ b/docs/reviews/Sprint_Review_Protocol_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\itp-minigames\docs\reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41675E3-8FC3-4448-BD73-DF2AC4B91C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD08A777-1FF6-4B43-A14E-47E18CDFD255}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -117,13 +117,22 @@
   </si>
   <si>
     <t>06.04.2021 - 13.04.2021</t>
+  </si>
+  <si>
+    <t>Front Page</t>
+  </si>
+  <si>
+    <t>Forum</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +178,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +227,12 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -419,7 +447,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -436,28 +464,9 @@
     <xf numFmtId="46" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="38" fontId="4" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="46" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -475,6 +484,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,9 +508,24 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="6" fillId="7" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
@@ -812,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3C726-37E9-451B-9308-D99ECF6E7468}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -833,28 +863,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
@@ -868,108 +898,108 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27">
+      <c r="B4" s="21"/>
+      <c r="C4" s="24">
         <v>2</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="29">
+      <c r="B6" s="23"/>
+      <c r="C6" s="26">
         <v>31</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="10" t="s">
         <v>23</v>
       </c>
@@ -981,38 +1011,38 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="11">
         <v>10</v>
       </c>
       <c r="I12" s="11">
-        <f>C17</f>
-        <v>5</v>
-      </c>
-      <c r="J12" s="12">
+        <f>C20</f>
+        <v>16</v>
+      </c>
+      <c r="J12" s="37">
         <f>I12-H12</f>
-        <v>-5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -1033,10 +1063,10 @@
       <c r="F15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="34"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
@@ -1048,7 +1078,7 @@
       <c r="C16" s="6">
         <v>5</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="12">
         <v>0.20069444444444443</v>
       </c>
       <c r="E16" s="2">
@@ -1057,33 +1087,118 @@
       <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5">
-        <f>SUM(C16,)</f>
+      <c r="A17" s="7">
+        <v>2</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.40625</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="6">
         <v>5</v>
       </c>
-      <c r="D17" s="9">
-        <f>SUM(D16,)</f>
-        <v>0.20069444444444443</v>
-      </c>
-      <c r="E17" s="5">
-        <f ca="1">COUNT(E16:E17)</f>
+      <c r="D19" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
         <v>0</v>
       </c>
-      <c r="F17" s="5">
-        <f ca="1">COUNT(F16:F17)</f>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5">
+        <f>SUM(C16,C17,C18,C19)</f>
+        <v>16</v>
+      </c>
+      <c r="D20" s="9">
+        <f>SUM(D16,D17,D18,D19)</f>
+        <v>1.0652777777777778</v>
+      </c>
+      <c r="E20" s="5">
+        <f ca="1">COUNT(E16:E20)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="F20" s="5">
+        <f ca="1">COUNT(F16:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="36"/>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="25">
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A1:I2"/>
@@ -1100,12 +1215,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>